<commit_message>
Updated excel file with address
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/framework/test/test_data.xlsx
+++ b/Automation/src/main/java/framework/test/test_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahanmelikyan/Documents/workspace/heal-qa-automation/Automation/src/main/java/framework/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian.rosu/heal-qa-automation/Automation/src/main/java/framework/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15980" windowHeight="12520" tabRatio="991"/>
+    <workbookView xWindow="2280" yWindow="900" windowWidth="38400" windowHeight="19600" tabRatio="991" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Key</t>
   </si>
@@ -125,6 +125,48 @@
   </si>
   <si>
     <t>vahan+qatest@heal.com</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>1 Market St</t>
+  </si>
+  <si>
+    <t>AddressType</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Establishment</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>HOME</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>gate code 4235</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
@@ -479,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -545,6 +587,72 @@
       </c>
       <c r="B7">
         <v>4839</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -564,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Added method for delete patient Added address on test_data.xlsx Added ops visits page Other clean-ups
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/framework/test/test_data.xlsx
+++ b/Automation/src/main/java/framework/test/test_data.xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian.rosu/heal-qa-automation/Automation/src/main/java/framework/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="19680" tabRatio="991"/>
   </bookViews>
   <sheets>
-    <sheet name="Account" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Patient" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Card" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Account" sheetId="1" r:id="rId1"/>
+    <sheet name="Patient" sheetId="2" r:id="rId2"/>
+    <sheet name="Card" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -22,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Key</t>
   </si>
@@ -115,18 +125,52 @@
   </si>
   <si>
     <t>Visa</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>AddressType</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Establishment</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>1 Market St</t>
+  </si>
+  <si>
+    <t>HOME</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>gate code 4235</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="166" formatCode="@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -134,29 +178,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
@@ -186,7 +215,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -194,77 +223,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -323,30 +301,296 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.63775510204082"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -354,62 +598,117 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>4839</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="mihaix16@heal.com"/>
+    <hyperlink ref="B4" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
@@ -417,24 +716,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.63775510204082"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,73 +733,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="B2" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>4753</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -517,12 +808,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="patientx@heal.com"/>
+    <hyperlink ref="B5" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
@@ -530,24 +820,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.63775510204082"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,51 +837,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3">
         <v>2022</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>314</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Finish book visit from OPS - added methods for avery step in Add visit module - added state and phone in test data - fixed selectByValue method - updated elements on OPS create visit page
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/framework/test/test_data.xlsx
+++ b/Automation/src/main/java/framework/test/test_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahanmelikyan/Documents/workspace/heal-qa-automation/Automation/src/main/java/framework/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian.rosu/qa-automation/Automation/src/main/java/framework/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19680" tabRatio="991"/>
+    <workbookView xWindow="38400" yWindow="440" windowWidth="38400" windowHeight="21160" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>Key</t>
   </si>
@@ -161,6 +161,33 @@
   </si>
   <si>
     <t>gate code 4235</t>
+  </si>
+  <si>
+    <t>MemberId</t>
+  </si>
+  <si>
+    <t>GroupId</t>
+  </si>
+  <si>
+    <t>COST_ESTIMATES_025</t>
+  </si>
+  <si>
+    <t>BC001</t>
+  </si>
+  <si>
+    <t>Payer</t>
+  </si>
+  <si>
+    <t>Anthem Blue Cross</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>California</t>
   </si>
 </sst>
 </file>
@@ -582,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -647,7 +674,7 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>4839</v>
+        <v>90210</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
@@ -704,6 +731,22 @@
       </c>
       <c r="B14" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15">
+        <v>2015555555</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -721,13 +764,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
@@ -783,7 +829,7 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>4753</v>
+        <v>90210</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
@@ -808,6 +854,38 @@
       </c>
       <c r="B10" s="7" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14">
+        <v>2015555555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added book visit with promo codes [ops] Added book visit with insurance [ops] Methods for search and select user, patient, address Added comments for tests Added new function for scroll page
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/framework/test/test_data.xlsx
+++ b/Automation/src/main/java/framework/test/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="440" windowWidth="38400" windowHeight="21160" tabRatio="991"/>
+    <workbookView xWindow="38400" yWindow="440" windowWidth="38400" windowHeight="19640" tabRatio="991" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>